<commit_message>
added logic for shippable
</commit_message>
<xml_diff>
--- a/Stage 2/Week 3/ecommerce methods.xlsx
+++ b/Stage 2/Week 3/ecommerce methods.xlsx
@@ -174,12 +174,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -194,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -205,6 +211,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H27" activeCellId="4" sqref="H19 H15 H11 H24 H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,7 +646,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H11" t="s">
+      <c r="H11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I11" s="3" t="s">
@@ -682,7 +689,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" t="s">
+      <c r="H15" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I15" s="3" t="s">
@@ -721,7 +728,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H19" t="s">
+      <c r="H19" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I19" s="3" t="s">
@@ -762,7 +769,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H24" t="s">
+      <c r="H24" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I24" s="3" t="s">
@@ -796,7 +803,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H27" t="s">
+      <c r="H27" s="4" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>